<commit_message>
Deaths have been implemented.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="705" windowWidth="28695" windowHeight="12540"/>
+    <workbookView xWindow="120" yWindow="1305" windowWidth="28695" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>id</t>
   </si>
@@ -60,6 +60,18 @@
   </si>
   <si>
     <t>Я продолжал стучать в дверь. Я подошел к входной двери постучал в неё. Из-за двери послышался голос: “ Ты человек? ”. Я ответил, что я человек и меня впустили внутрь.</t>
+  </si>
+  <si>
+    <t>“Ты как здесь оказался, у нас в деревне даже 100-а жителей не наберется, все друг друга в лицо знают” – спросил у меня выживший – “ Тоже не успел на эвакуацию?”. Мы сели за стол, этот выживший налил чай и попросил мне объяснить, кто я и как я здесь оказался. Моего собеседника звали Виктор. Я ничего не понимал, я попытался ему объяснить, что я турист, который был в недельном походе от одной деревни в другую. “Слушай, рассказываю для мяса, за те семь дней, которые ты был в своём походе, случилась эпидемия, которая поразила весь мир. Люди превратились в кровожадных тварей, которые жаждут тебя сожрать. Если так можно сказать случился обычный “Голливудский” зомби апокалипсис. Все города превратились в огромные рассадники зомби, там жизни нет. Все кто успел, эвакуировались из городов в деревни и сёла, но вирус добрался и до нас, не знаю насчёт остальных стран, но Россия уже почти полностью пала, последние новости, которые я смог увидеть были в четверг, на них говорилось, что вспышки вируса были замечены во всех странах. Они объявили, что эвакуация происходит по некоторым шоссе, в том числе и тому, которое располагается недалеко от этой деревни. Но из-за того что автобусы, которые приехали в эту деревню привлекли зомби с округи, не все успели эвакуироваться и их либо сожрали, либо они смогли убежать в неизвестном направлении, как я. Думаю что если идти вдоль шоссе то мы сможем дойти до военного блокпоста, так как звук привлекает их, а значит они должны последовать за автобусами ”. Я был шокирован услышанным, но когда с чердака избушки, в которой мы были, я увидел, как зомби пожирали чей-то труп, то мне просто пришлось поверить в данную историю. Мой спаситель был мужчина возраста около 45 лет, по его словам он был ветераном Чеченской войны, и поэтому навыки, полученные им на войне, помогли ему выжить.. Он предложил мне попробовать добраться до военного блокпоста, потому что это единственный способ выжить. Мы собрали все припасы, которые есть у Виктора. Самое главное, что Виктор был охотником и в его запасе имелись блочный лук, арбалет  и боеприпасы к ним. Он дал мне на вооружение арбалет, а сам взял лук, так как сказал, что с арбалетом мне будет обращаться легче, чем с луком. Но как только мы вышли на улицу, нам встретилось трое ходячих мертвецов. Что же нам с ними делать?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Пока мы собирали припасы, Виктор объяснил мне как пользоваться арбалетом из-за чего убить зомби мне не составило труда, особенно под надзором Виктора. Мы пошли к выходу из деревни, как Виктор и предполагал звуки моторов эвакуационных автобусов, уманили часть зомби за собой, а остальную привлекли за собой не успевшие  эвакуироваться люди. Из-за чего нам не составило труда выйти до шоссе и пойти по нему. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Мы спрятались за углом здания и стали кидать камни в сторону зомби. Поначалу таким трюком зомби не приманивались, но на один из камней они отреагировали все втроём, двое из них даже побежали. Виктор ловким движением рук выстрелил из лука и убил одного из них, но паника сыграла свою роль, и мой арбалет дал осечку зомби повалил меня и укусил за шею, я кричал от боли очень громко. Виктор убил оставшихся остальных зомби, он успокоил меня тем, что по его наблюдениям, укус заражает, только если тебя укусил кровавый зомби, но было уже слишком. На мои крики сбежалось около 30 зомби, мы пытались отстреливаться, но нам не хватило времени на то, чтобы убить их всех, они повалили нас и загрызли. Смерть </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Мы решили обойти их по-тихому, что не составило труда. Мы пошли к выходу из деревни, как Виктор и предполагал звуки моторов эвакуационных автобусов, уманили часть зомби за собой, а остальную привлекли за собой не успевшие  эвакуироваться люди. Из-за чего нам не составило труда выйти до шоссе и пойти по нему. </t>
   </si>
 </sst>
 </file>
@@ -96,9 +108,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -403,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,10 +529,37 @@
       <c r="A12">
         <v>20</v>
       </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>22</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
System of life has been implemented. Game for restoring of life is in progress.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="1305" windowWidth="28695" windowHeight="12540"/>
+    <workbookView xWindow="120" yWindow="1905" windowWidth="28695" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>id</t>
   </si>
@@ -72,6 +72,18 @@
   </si>
   <si>
     <t xml:space="preserve">Мы решили обойти их по-тихому, что не составило труда. Мы пошли к выходу из деревни, как Виктор и предполагал звуки моторов эвакуационных автобусов, уманили часть зомби за собой, а остальную привлекли за собой не успевшие  эвакуироваться люди. Из-за чего нам не составило труда выйти до шоссе и пойти по нему. </t>
+  </si>
+  <si>
+    <t>Мы шли по шоссе целый день, попутно говоря о данной ситуации, зомби встречались, но встречались очень редко и обойти их или убить не составляло труда. Уже начало смеркаться. Мы думали о ночлеге, так как за день дороги очень устали. Но вдруг вдалеке зажглись огни. Несомненно, это был военный блокпост. Это было понятно, потому что были видны четыре вышки, которые светили прожекторами на прилежавшую территорию.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Мы расставили платки недалеко от шоссе, так как боялись потеряться. Мы решили, что первый на стрёме стою я. Прошло уже 3 часа. Уже была очередь сменяться. Но из-за своей сонливости я не заметил, как зомби подошёл ко мне и укусил. Чувствовалась огромная боль в моей руке. Мне удалось убить его, но на мои крики стекались зомби из леса. Пока Виктор вставал на меня напали уже двое ходячих. Мы отбились и от них. Но нас уже окружили около дюжины зомби. И сначала меня, а потом и Виктора повалили и загрызли. Смерть </t>
+  </si>
+  <si>
+    <t>Мы сразу забыли о ночлеге и решили марш броском пройти это расстояние. Но приближаясь к блокпосту количество, зомби начало увеличиваться. Поначалу мы убивали их с помощью охотничьих ножей, но скоро стало совсем темно. Мы не заметили, как нас окружила толпа из примерно 30 зомби, благо они поначалу не замечали нас и время на то, чтобы придумать план действий был.</t>
+  </si>
+  <si>
+    <t>Мы решили просто пробежать их. Поначалу у нас всё складывалось отлично, но из-за кромешной тьмы Виктор не увидел зомби и запнулся об него, у которого не было ног. Помочь ему мне сразу не удалось, так как мне загородили проход к нему три зомби.</t>
   </si>
 </sst>
 </file>
@@ -418,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,6 +567,38 @@
       </c>
       <c r="B15" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>42</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>52</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Last events have been added. Plot seems to be ready. Player skills are in progress.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="1905" windowWidth="28695" windowHeight="12540"/>
+    <workbookView xWindow="120" yWindow="2505" windowWidth="28695" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>id</t>
   </si>
@@ -83,7 +83,34 @@
     <t>Мы сразу забыли о ночлеге и решили марш броском пройти это расстояние. Но приближаясь к блокпосту количество, зомби начало увеличиваться. Поначалу мы убивали их с помощью охотничьих ножей, но скоро стало совсем темно. Мы не заметили, как нас окружила толпа из примерно 30 зомби, благо они поначалу не замечали нас и время на то, чтобы придумать план действий был.</t>
   </si>
   <si>
-    <t>Мы решили просто пробежать их. Поначалу у нас всё складывалось отлично, но из-за кромешной тьмы Виктор не увидел зомби и запнулся об него, у которого не было ног. Помочь ему мне сразу не удалось, так как мне загородили проход к нему три зомби.</t>
+    <t xml:space="preserve">Мы решили просто пробежать их. Поначалу у нас всё складывалось отлично, но из-за кромешной тьмы Виктор не увидел зомби, у которого не было ног, и запнулся об него. Помочь ему мне сразу не удалось, так как мне загородили проход к нему три зомби. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Из-за того, что я тренировался с арбалетом на зомби ранее, у меня без труда получилось убить их и  помочь Виктору скинуть зомби с себя. По итогу мы смогли пробежать через оставшихся зомби и прийти на блокпост. В нас уже было хотели стрелять, так как подумали, что мы можем быть зомби. Но мы подали жесты руками и нас определили как людей. Нас пустили на военный блокпост и повели на медицинский осмотр. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Я уже не помнил слова Виктора о том, как стрелять с арбалета. Я смог убить одного, но из-за долгой перезарядки и последующего за ним промаха на меня сзади успел накинуться зомби и повалить. Сил во мне уже не оставалось, и меня загрызли. Смерть </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Из-за того, что у меня ранее был опыт в бесшумных убийствах зомби, мне не составило труда сделать это еще раз. Я убил тех трёх зомби, после чего помог Виктору. По итогу мы смогли пробежать через оставшихся зомби и прийти на блокпост. В нас уже было хотели стрелять, так как подумали, что мы можем быть зомби. Но мы подали жесты руками и нас определили как людей. Нас пустили на военный блокпост и повели на медицинский осмотр. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Я решил попробовать убить их бесшумно. Но подходя к ним, я издавал слишком много шума. Они обернулись и разом накинулись на меня, после чего загрызли. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Мы с Виктором  забрались на небольшую газель, и мы начали отстреливаться. В боезапасе было  10 стрел и 12 арбалетных болтов. На прошлой троице зомби еще в деревне я научился правильно прицеливать и перезаряжаться. Все стрелы и болты, которые мы выпускали, попадали точно в цель. Оставшихся пятерых зомби мы смогли убить с помощью ножей. Мы спустились с машины и пошли до военного блокпоста. В нас уже было хотели стрелять, так как подумали, что мы можем быть зомби. Но мы подали жесты руками и нас определили как людей. Нас пустили на военный блокпост и повели на медицинский осмотр. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Мы с Виктором  забрались на небольшую газель и начали отстреливаться. В боезапасе было  10 стрел и 15 арбалетных болтов. Я плохо помнил инструктаж Виктора и не смог попасть всеми болтами арбалета из-за нервозности и тремора в руках. Их оставалось около 15. Но вдруг они смогли подняться на капот, а в последующем и на крышу. Нам ничего не оставалось, кроме того, что прыгать с крыши газели. Виктор смог спрыгнуть и сделать кувырок для смягчения падения, а я, прыгая с крыши, повредил себе ногу и не смог вовремя убежать. На меня накинулись зомби и загрызли. Смерть </t>
+  </si>
+  <si>
+    <t>Мы решили прокрасться через них по-тихому. К счастью у нас уже был опыт в убийстве зомби со спины. Нам не составило труда кого-то убить, а кого-то обойти. Так что для нас это не было сложным испытанием. Мы продолжили путь до блокпоста. В нас уже было хотели стрелять, так как подумали, что мы можем быть зомби. Но мы подали жесты руками и нас определили как людей. Нас пустили на военный блокпост и повели на медицинский осмотр.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Мы решили прокрасться через них по-тихому. Но мы никогда не оказывались в такой ситуации, поэтому, что делать мы не знали. Нас охватила легкая паника. А тем временем зомби были все ближе и больше. Еще немного подумав, мы все же решились идти. Мы начали тихонько обходить зомби, но из-за нервности мы совершили ошибку. В темноте Виктор не заметил труп и запнулся об него. От неожиданности он охнул. Зомби заметили нас и начали окружать. Их стало еще больше, и мы не смогли выбраться. Нас загрызли. </t>
+  </si>
+  <si>
+    <t>death</t>
   </si>
 </sst>
 </file>
@@ -430,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,7 +470,7 @@
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -456,8 +483,11 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -465,7 +495,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -473,7 +503,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>11</v>
       </c>
@@ -481,7 +511,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>12</v>
       </c>
@@ -489,7 +519,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>13</v>
       </c>
@@ -497,7 +527,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -505,7 +535,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -513,7 +543,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>31</v>
       </c>
@@ -521,7 +551,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>32</v>
       </c>
@@ -529,7 +559,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>33</v>
       </c>
@@ -537,7 +567,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>20</v>
       </c>
@@ -545,7 +575,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>21</v>
       </c>
@@ -553,7 +583,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>22</v>
       </c>
@@ -561,7 +591,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>23</v>
       </c>
@@ -569,7 +599,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>30</v>
       </c>
@@ -599,6 +629,70 @@
       </c>
       <c r="B19" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>611</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>612</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>621</v>
+      </c>
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>622</v>
+      </c>
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>5111</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>5112</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>5331</v>
+      </c>
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>5332</v>
+      </c>
+      <c r="B27" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>